<commit_message>
change background and color style
</commit_message>
<xml_diff>
--- a/server/data/users.xlsx
+++ b/server/data/users.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/collin/Desktop/lottery/server/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/collin/Desktop/lottery_backup/server/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9300DAB-FE01-604E-9C88-45A1164A4880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{319FE47A-50DF-7943-96BB-EA529C359512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="74">
   <si>
     <t>工号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -46,108 +46,6 @@
     <t>ADA</t>
   </si>
   <si>
-    <t>User 1</t>
-  </si>
-  <si>
-    <t>User 2</t>
-  </si>
-  <si>
-    <t>User 3</t>
-  </si>
-  <si>
-    <t>User 4</t>
-  </si>
-  <si>
-    <t>User 5</t>
-  </si>
-  <si>
-    <t>User 6</t>
-  </si>
-  <si>
-    <t>User 7</t>
-  </si>
-  <si>
-    <t>User 8</t>
-  </si>
-  <si>
-    <t>User 9</t>
-  </si>
-  <si>
-    <t>User 10</t>
-  </si>
-  <si>
-    <t>User 11</t>
-  </si>
-  <si>
-    <t>User 12</t>
-  </si>
-  <si>
-    <t>User 13</t>
-  </si>
-  <si>
-    <t>User 14</t>
-  </si>
-  <si>
-    <t>User 15</t>
-  </si>
-  <si>
-    <t>User 16</t>
-  </si>
-  <si>
-    <t>User 17</t>
-  </si>
-  <si>
-    <t>User 18</t>
-  </si>
-  <si>
-    <t>User 19</t>
-  </si>
-  <si>
-    <t>User 20</t>
-  </si>
-  <si>
-    <t>User 21</t>
-  </si>
-  <si>
-    <t>User 22</t>
-  </si>
-  <si>
-    <t>User 23</t>
-  </si>
-  <si>
-    <t>User 24</t>
-  </si>
-  <si>
-    <t>User 25</t>
-  </si>
-  <si>
-    <t>User 26</t>
-  </si>
-  <si>
-    <t>User 27</t>
-  </si>
-  <si>
-    <t>User 28</t>
-  </si>
-  <si>
-    <t>User 29</t>
-  </si>
-  <si>
-    <t>User 30</t>
-  </si>
-  <si>
-    <t>User 31</t>
-  </si>
-  <si>
-    <t>User 32</t>
-  </si>
-  <si>
-    <t>User 33</t>
-  </si>
-  <si>
-    <t>User 34</t>
-  </si>
-  <si>
     <t>000002</t>
   </si>
   <si>
@@ -245,13 +143,121 @@
   </si>
   <si>
     <t>000034</t>
+  </si>
+  <si>
+    <t>000035</t>
+  </si>
+  <si>
+    <t>Javen Deng </t>
+  </si>
+  <si>
+    <t>Aaron Xuehui Song</t>
+  </si>
+  <si>
+    <t>Alex Kexin Li</t>
+  </si>
+  <si>
+    <t>Alex Sheng Zhong </t>
+  </si>
+  <si>
+    <t>Alex Tianyun Wang</t>
+  </si>
+  <si>
+    <t>Alger Zhenhai Wu</t>
+  </si>
+  <si>
+    <t>Andrew Zhengyu He</t>
+  </si>
+  <si>
+    <t>Beer Bowei Li</t>
+  </si>
+  <si>
+    <t>Charles He</t>
+  </si>
+  <si>
+    <t>Daniel Weiyang Huo</t>
+  </si>
+  <si>
+    <t>Davis Songyou Zhong</t>
+  </si>
+  <si>
+    <t>Doris Haixia Yu </t>
+  </si>
+  <si>
+    <t>Fangzheng Xu</t>
+  </si>
+  <si>
+    <t>Feng Zong </t>
+  </si>
+  <si>
+    <t>Guohao Wang </t>
+  </si>
+  <si>
+    <t>Huancheng Lu </t>
+  </si>
+  <si>
+    <t>Jack Guangjie Huang</t>
+  </si>
+  <si>
+    <t>Jacky Zhihuang Zhang</t>
+  </si>
+  <si>
+    <t>Jade Jiepeng Li </t>
+  </si>
+  <si>
+    <t>Jay Jie Pan </t>
+  </si>
+  <si>
+    <t>Joey Jieyu Chen </t>
+  </si>
+  <si>
+    <t>Keyshawn Xianghui Kong</t>
+  </si>
+  <si>
+    <t>Liese Cong Lu </t>
+  </si>
+  <si>
+    <t>Chen Lu</t>
+  </si>
+  <si>
+    <t>Mike Mengyan Dong </t>
+  </si>
+  <si>
+    <t>Mike Weihao Luo </t>
+  </si>
+  <si>
+    <t>Raymond Xinyu Zheng</t>
+  </si>
+  <si>
+    <t>Renchuan Xiao </t>
+  </si>
+  <si>
+    <t>Syed Muzamil Hussain</t>
+  </si>
+  <si>
+    <t>Taylor Qi Huang </t>
+  </si>
+  <si>
+    <t>Yann Jiyan Guo </t>
+  </si>
+  <si>
+    <t>Zizhao Zhang </t>
+  </si>
+  <si>
+    <t>Zuying Hu </t>
+  </si>
+  <si>
+    <t>Kai He </t>
+  </si>
+  <si>
+    <t>Wenjie Liu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,6 +293,12 @@
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -332,7 +344,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -349,6 +361,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -667,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="164" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.6640625" defaultRowHeight="18"/>
@@ -691,8 +706,8 @@
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+      <c r="B2" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>4</v>
@@ -700,10 +715,10 @@
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>4</v>
@@ -711,10 +726,10 @@
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>4</v>
@@ -722,10 +737,10 @@
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>4</v>
@@ -733,10 +748,10 @@
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>4</v>
@@ -744,10 +759,10 @@
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>4</v>
@@ -755,10 +770,10 @@
     </row>
     <row r="8" spans="1:3" ht="19">
       <c r="A8" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>4</v>
@@ -766,10 +781,10 @@
     </row>
     <row r="9" spans="1:3" ht="19">
       <c r="A9" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>4</v>
@@ -777,10 +792,10 @@
     </row>
     <row r="10" spans="1:3" ht="19">
       <c r="A10" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>4</v>
@@ -788,10 +803,10 @@
     </row>
     <row r="11" spans="1:3" ht="19">
       <c r="A11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>4</v>
@@ -799,10 +814,10 @@
     </row>
     <row r="12" spans="1:3" ht="19">
       <c r="A12" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>4</v>
@@ -810,10 +825,10 @@
     </row>
     <row r="13" spans="1:3" ht="19">
       <c r="A13" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>4</v>
@@ -821,10 +836,10 @@
     </row>
     <row r="14" spans="1:3" ht="19">
       <c r="A14" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>4</v>
@@ -832,10 +847,10 @@
     </row>
     <row r="15" spans="1:3" ht="19">
       <c r="A15" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>4</v>
@@ -843,10 +858,10 @@
     </row>
     <row r="16" spans="1:3" ht="19">
       <c r="A16" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>4</v>
@@ -854,10 +869,10 @@
     </row>
     <row r="17" spans="1:3" ht="19">
       <c r="A17" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>4</v>
@@ -865,10 +880,10 @@
     </row>
     <row r="18" spans="1:3" ht="19">
       <c r="A18" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>4</v>
@@ -876,10 +891,10 @@
     </row>
     <row r="19" spans="1:3" ht="19">
       <c r="A19" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>4</v>
@@ -887,10 +902,10 @@
     </row>
     <row r="20" spans="1:3" ht="19">
       <c r="A20" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>4</v>
@@ -898,10 +913,10 @@
     </row>
     <row r="21" spans="1:3" ht="19">
       <c r="A21" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>4</v>
@@ -909,10 +924,10 @@
     </row>
     <row r="22" spans="1:3" ht="19">
       <c r="A22" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>4</v>
@@ -920,10 +935,10 @@
     </row>
     <row r="23" spans="1:3" ht="19">
       <c r="A23" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>4</v>
@@ -931,10 +946,10 @@
     </row>
     <row r="24" spans="1:3" ht="19">
       <c r="A24" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>4</v>
@@ -942,10 +957,10 @@
     </row>
     <row r="25" spans="1:3" ht="19">
       <c r="A25" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>4</v>
@@ -953,10 +968,10 @@
     </row>
     <row r="26" spans="1:3" ht="19">
       <c r="A26" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>4</v>
@@ -964,10 +979,10 @@
     </row>
     <row r="27" spans="1:3" ht="19">
       <c r="A27" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>4</v>
@@ -975,10 +990,10 @@
     </row>
     <row r="28" spans="1:3" ht="19">
       <c r="A28" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>4</v>
@@ -986,10 +1001,10 @@
     </row>
     <row r="29" spans="1:3" ht="19">
       <c r="A29" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>4</v>
@@ -997,10 +1012,10 @@
     </row>
     <row r="30" spans="1:3" ht="19">
       <c r="A30" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>4</v>
@@ -1008,10 +1023,10 @@
     </row>
     <row r="31" spans="1:3" ht="19">
       <c r="A31" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>4</v>
@@ -1019,10 +1034,10 @@
     </row>
     <row r="32" spans="1:3" ht="19">
       <c r="A32" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>4</v>
@@ -1030,10 +1045,10 @@
     </row>
     <row r="33" spans="1:3" ht="19">
       <c r="A33" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>70</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>4</v>
@@ -1041,10 +1056,10 @@
     </row>
     <row r="34" spans="1:3" ht="19">
       <c r="A34" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>4</v>
@@ -1052,19 +1067,25 @@
     </row>
     <row r="35" spans="1:3" ht="19">
       <c r="A35" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B35" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="19">
+      <c r="A36" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="3"/>
+      <c r="B36" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="2"/>

</xml_diff>